<commit_message>
Entwürfe zum Großteil angepasst
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Julian Halbmayr/DA_Stundenaufzeichnungen-JulianHalbmayr.xlsx
+++ b/Stundenaufzeichnungen/Julian Halbmayr/DA_Stundenaufzeichnungen-JulianHalbmayr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\HTL_Waidhofen\Diplomarbeit\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Julian Halbmayr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E99CCA-D8A6-4021-8593-66323A36F6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B236787-1AB0-4859-A061-E8B9B48E664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Login/ Registrierungsseiten  Entwurf überarbeitet, Pilotenseite Entwurf fertiggestellt</t>
+  </si>
+  <si>
+    <t>Besprechung mit Gabriel</t>
+  </si>
+  <si>
+    <t>Besprechung mit Gabriel wegen dem Status Meeting am folgenden Tag (19.07.2025), Entwurfe angepasst, Skizzen und Notizen erstellt</t>
+  </si>
+  <si>
+    <t>Erstes Meeting mit Michael Maurer, Ort: Haus von Michael Maurer, Design Entwürfe hergezeigt, Verbesserungen des aktuellen Zustands besprochen</t>
+  </si>
+  <si>
+    <t>Besprechungsprotokoll mit Gabriel Deiac geschreiben</t>
   </si>
 </sst>
 </file>
@@ -235,12 +247,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -579,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,401 +633,425 @@
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="5">
         <v>45829</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="5">
         <v>45839</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="5">
         <v>45840</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="5">
         <v>45841</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="5">
         <v>45842</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
+      <c r="A16" s="5">
+        <v>45847</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="5">
+        <v>45856</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="5">
+        <v>45857</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="5">
+        <v>45857</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>17</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,524 +1067,452 @@
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>17</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
       <c r="G58" s="4"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
       <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
       <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
       <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
       <c r="G71" s="4"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
       <c r="G72" s="4"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
       <c r="G73" s="4"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
       <c r="G74" s="4"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
       <c r="G75" s="4"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
       <c r="G76" s="4"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
       <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
       <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
       <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
       <c r="G80" s="4"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
       <c r="G81" s="4"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
       <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
       <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
       <c r="G84" s="4"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
       <c r="G85" s="4"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
       <c r="G86" s="4"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
       <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
       <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
       <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
       <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
       <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
       <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
       <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
       <c r="G94" s="4"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
       <c r="G95" s="4"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
       <c r="G96" s="4"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
       <c r="G97" s="4"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
       <c r="G98" s="4"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>17</v>
+        <v>22.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B97:F97"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B49:F49"/>
@@ -1565,6 +1529,78 @@
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1573,18 +1609,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1732,6 +1768,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D31C018F-2049-43E6-BD93-F5C295BFDE2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1744,14 +1788,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e3f71932-39fd-488a-9e11-aeac0423eab6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AF60E-0EF1-43CF-BBE9-09CB79E28327}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Entwürfe überarbeitet + Filteranischten erstellt
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnungen/Julian Halbmayr/DA_Stundenaufzeichnungen-JulianHalbmayr.xlsx
+++ b/Stundenaufzeichnungen/Julian Halbmayr/DA_Stundenaufzeichnungen-JulianHalbmayr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\HTL_Waidhofen\Diplomarbeit\Digitales-Flugplatzmanagement\Stundenaufzeichnungen\Julian Halbmayr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B236787-1AB0-4859-A061-E8B9B48E664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC0856-1798-463E-A6F1-E16F38D75531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Stundenaufzeichnungen für Diplomarbeit</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Besprechungsprotokoll mit Gabriel Deiac geschreiben</t>
+  </si>
+  <si>
+    <t>Besprechung mit Gabriel wegen Entwürfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entwürfe überarbeitet + Filteransichten erstellt </t>
   </si>
 </sst>
 </file>
@@ -591,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,22 +786,34 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5">
+        <v>45862</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="5">
+        <v>45863</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
@@ -1051,7 +1069,7 @@
       <c r="F49" s="10"/>
       <c r="G49" s="3">
         <f>SUM(G11:G48)</f>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1089,7 +1107,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="4">
         <f>G49</f>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,7 +1526,7 @@
       <c r="F99" s="6"/>
       <c r="G99" s="3">
         <f>SUM(G53:G98)</f>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>